<commit_message>
only english language is supported properly
</commit_message>
<xml_diff>
--- a/fio.xlsx
+++ b/fio.xlsx
@@ -425,10 +425,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -474,14 +474,168 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>New test</t>
+          <t>Welcome</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ﾐ湲τひｸﾐｽ</t>
+          <t>Today</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Vasya</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Андрей</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Мария</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Дрон</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Roman</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Obama</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Алексей</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Владимир</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Кирилл</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Далгат</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ﾐ侑ｽﾐｽﾐｾﾐｺﾐｵﾐｽﾑひｸ</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Ivanov Ivan</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Irtuganov Nickolay</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Vasiliev Dmitrie</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Qwerty123</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Qwerty1234</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Qwerty</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Qwerty9876</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ﾐ籍ｱﾐｰﾐｽﾐｴﾐｾﾐｽ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Абхазия</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Alexandr</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Alex</t>
         </is>
       </c>
     </row>

</xml_diff>